<commit_message>
Report matching Spreadsheet Complete
</commit_message>
<xml_diff>
--- a/public/downloads/Template Files/Invoices Back Ordered Report Result.xlsx
+++ b/public/downloads/Template Files/Invoices Back Ordered Report Result.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Meteor\spreadsheet_template\Final\Template Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD4CC3C-DA01-45E3-8784-078AC4BBD8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Invoices Back Ordered Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Raw Data'!$A$1:$CZ$20</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,15 +28,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{14EAC24B-6B96-4FCC-B228-06B8D6C99757}" keepAlive="1" name="Query - TInvoiceList?IgnoreDates=true&amp;Search=Deleted%20!%3D%20true&amp;OrderBy=SaleID%20desc" description="Connection to the 'TInvoiceList?IgnoreDates=true&amp;Search=Deleted%20!%3D%20true&amp;OrderBy=SaleID%20desc' query in the workbook." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Query - TInvoiceList?IgnoreDates=true&amp;Search=Deleted%20!%3D%20true&amp;OrderBy=SaleID%20desc" description="Connection to the 'TInvoiceList?IgnoreDates=true&amp;Search=Deleted%20!%3D%20true&amp;OrderBy=SaleID%20desc' query in the workbook." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;TInvoiceList?IgnoreDates=true&amp;Search=Deleted%20!%3D%20true&amp;OrderBy=SaleID%20desc&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [TInvoiceList?IgnoreDates=true&amp;Search=Deleted%20!%3D%20true&amp;OrderBy=SaleID%20desc]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="262">
   <si>
     <t>T.InvoiceDocNumber</t>
   </si>
@@ -825,15 +824,57 @@
   <si>
     <t>Comments</t>
   </si>
+  <si>
+    <t>Report To</t>
+  </si>
+  <si>
+    <t>Received By</t>
+  </si>
+  <si>
+    <t>2023-01-13 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2022-12-19 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2022-06-29 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2022-03-30 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2021-12-07 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2021-10-08 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2021-04-28 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2021-01-13 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2020-10-07 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2020-09-30 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2020-08-05 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>2020-09-03 00:00:00 Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +889,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
@@ -874,16 +922,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -901,7 +961,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -915,7 +974,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -929,7 +987,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -943,7 +1000,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -957,7 +1013,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -971,7 +1026,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -985,7 +1039,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -999,7 +1052,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1013,7 +1065,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1027,7 +1078,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1041,7 +1091,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1055,7 +1104,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1069,7 +1117,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1083,7 +1130,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1097,7 +1143,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1111,7 +1156,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1125,7 +1169,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1139,7 +1182,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1153,7 +1195,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1167,7 +1208,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1181,7 +1221,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1195,7 +1234,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1209,7 +1247,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1223,7 +1260,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1237,7 +1273,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1251,7 +1286,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1265,7 +1299,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1279,7 +1312,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1293,7 +1325,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1307,7 +1338,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1321,7 +1351,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1335,7 +1364,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1349,7 +1377,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1363,7 +1390,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1377,7 +1403,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1391,7 +1416,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1405,7 +1429,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1419,7 +1442,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1433,7 +1455,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1447,7 +1468,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1461,7 +1481,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1475,7 +1494,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1489,7 +1507,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1503,7 +1520,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1517,7 +1533,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1531,7 +1546,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1545,7 +1559,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1559,7 +1572,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1573,7 +1585,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1587,7 +1598,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1601,7 +1611,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1615,7 +1624,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1629,7 +1637,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1643,7 +1650,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1657,7 +1663,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1671,7 +1676,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1685,7 +1689,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1699,7 +1702,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1713,7 +1715,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1727,7 +1728,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1741,7 +1741,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1755,7 +1754,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1769,7 +1767,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1783,7 +1780,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1797,7 +1793,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1811,7 +1806,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1825,7 +1819,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1839,7 +1832,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1853,7 +1845,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1867,7 +1858,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1881,7 +1871,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1895,7 +1884,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1909,7 +1897,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1923,7 +1910,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1937,7 +1923,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1951,7 +1936,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1965,7 +1949,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1979,7 +1962,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1993,7 +1975,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2007,7 +1988,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2021,7 +2001,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2035,7 +2014,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2049,7 +2027,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2063,7 +2040,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2077,7 +2053,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2091,7 +2066,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2105,7 +2079,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2119,7 +2092,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2133,7 +2105,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2147,7 +2118,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2161,7 +2131,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2175,7 +2144,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2189,7 +2157,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2203,7 +2170,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2217,7 +2183,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2231,7 +2196,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2245,7 +2209,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2259,7 +2222,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2273,7 +2235,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2287,7 +2248,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2301,7 +2261,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2315,7 +2274,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2329,7 +2287,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2343,7 +2300,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2357,7 +2313,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2371,7 +2326,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Segoe UI"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2389,7 +2343,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{2880905A-F1C5-45E8-B721-AD717E72D30E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="105">
     <queryTableFields count="104">
       <queryTableField id="1" name="T.InvoiceDocNumber" tableColumnId="105"/>
@@ -2502,113 +2456,113 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C0B9EFD5-1ED9-4543-986C-40E3DC51C0A0}" name="TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc" displayName="TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc" ref="A1:CZ20" tableType="queryTable" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
-  <autoFilter ref="A1:CZ20" xr:uid="{C0B9EFD5-1ED9-4543-986C-40E3DC51C0A0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc" displayName="TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc" ref="A1:CZ20" tableType="queryTable" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+  <autoFilter ref="A1:CZ20"/>
   <tableColumns count="104">
-    <tableColumn id="105" xr3:uid="{955A3F0C-0D91-4670-9E83-AEE1BB44AC5E}" uniqueName="105" name="T.InvoiceDocNumber" queryTableFieldId="1" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{C08592B9-7CD0-4F69-9C86-AA92E64F9434}" uniqueName="2" name="T.Account" queryTableFieldId="2" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{4C462813-56EC-4FFC-832A-8DD5B44A9053}" uniqueName="3" name="T.CustomerName" queryTableFieldId="3" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{976EB0C1-7FF8-48C4-96FF-E9180ACA59DB}" uniqueName="4" name="T.InvoiceTo" queryTableFieldId="4" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{E1D43FE3-5E32-4B88-8B68-F839EF263D91}" uniqueName="5" name="T.ShipTo" queryTableFieldId="5" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{3906B99C-2F26-4B8A-BE12-3D391B84E1D7}" uniqueName="6" name="T.PickupFrom" queryTableFieldId="6" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{7F6F82DB-3641-4211-B060-3FAC52E29D36}" uniqueName="7" name="T.SaleDate" queryTableFieldId="7" dataDxfId="97"/>
-    <tableColumn id="8" xr3:uid="{19ED3D15-4556-430B-BF2E-BAEA1FDE2290}" uniqueName="8" name="T.TotalTax" queryTableFieldId="8" dataDxfId="96"/>
-    <tableColumn id="9" xr3:uid="{85A93F3B-B399-4124-B83B-FE8040464EC3}" uniqueName="9" name="T.TotalAmount" queryTableFieldId="9" dataDxfId="95"/>
-    <tableColumn id="10" xr3:uid="{6AC8C162-ADB2-488F-8E31-00C9CFE2255D}" uniqueName="10" name="T.TotalAmountInc" queryTableFieldId="10" dataDxfId="94"/>
-    <tableColumn id="11" xr3:uid="{1FE17E2E-AA7A-4EC1-A97A-055D074F82A7}" uniqueName="11" name="T.TotalMarkup" queryTableFieldId="11" dataDxfId="93"/>
-    <tableColumn id="12" xr3:uid="{D02D1A68-47EC-41E8-B7D1-8CF6185B0FD5}" uniqueName="12" name="T.TotalDiscount" queryTableFieldId="12" dataDxfId="92"/>
-    <tableColumn id="13" xr3:uid="{0858283B-FAF9-4157-BCEB-D4FC7DCF1EBF}" uniqueName="13" name="T.EmployeeName" queryTableFieldId="13" dataDxfId="91"/>
-    <tableColumn id="14" xr3:uid="{461119A7-75D0-41E0-9DA2-8E2E5957D45F}" uniqueName="14" name="T.Class" queryTableFieldId="14" dataDxfId="90"/>
-    <tableColumn id="15" xr3:uid="{28D6A755-9DB4-47CD-91AF-23A0803F6248}" uniqueName="15" name="T.OrderNumber" queryTableFieldId="15" dataDxfId="89"/>
-    <tableColumn id="16" xr3:uid="{D97D9B9F-7198-455D-B9C3-0A85B8C7CE74}" uniqueName="16" name="T.PONumber" queryTableFieldId="16" dataDxfId="88"/>
-    <tableColumn id="17" xr3:uid="{9AE07AF4-5FB3-4373-BA23-0753A2FED08E}" uniqueName="17" name="T.ChequeNo" queryTableFieldId="17" dataDxfId="87"/>
-    <tableColumn id="18" xr3:uid="{4EAE03A6-71BA-4E30-B8C9-B66ADC10353A}" uniqueName="18" name="T.ShipDate" queryTableFieldId="18" dataDxfId="86"/>
-    <tableColumn id="19" xr3:uid="{192C5E4F-D6AC-46BE-B2F0-12A677F5CCED}" uniqueName="19" name="T.FutureSO" queryTableFieldId="19" dataDxfId="85"/>
-    <tableColumn id="20" xr3:uid="{7F6C22E2-F813-4780-8F3D-83EE2E3E3622}" uniqueName="20" name="T.DueDate" queryTableFieldId="20" dataDxfId="84"/>
-    <tableColumn id="21" xr3:uid="{BBDE9811-18F2-47CD-9F23-5E814594E185}" uniqueName="21" name="T.ConNote" queryTableFieldId="21" dataDxfId="83"/>
-    <tableColumn id="22" xr3:uid="{BB9EDC41-7B43-48EE-9FB2-C08560FA3EAE}" uniqueName="22" name="T.Comments" queryTableFieldId="22" dataDxfId="82"/>
-    <tableColumn id="23" xr3:uid="{503E28AE-6CA3-4A16-B2CB-4B102C161EEE}" uniqueName="23" name="T.Shipping" queryTableFieldId="23" dataDxfId="81"/>
-    <tableColumn id="24" xr3:uid="{9B3105A7-E68C-4F50-BD46-A37159D982CC}" uniqueName="24" name="T.Terms" queryTableFieldId="24" dataDxfId="80"/>
-    <tableColumn id="25" xr3:uid="{0A7CDCD8-733D-48CE-BCBE-0FDB49DCF978}" uniqueName="25" name="T.PayMethod" queryTableFieldId="25" dataDxfId="79"/>
-    <tableColumn id="26" xr3:uid="{7C731519-5A21-4AE8-BB60-DA3F8BC56F51}" uniqueName="26" name="T.PayDueDate" queryTableFieldId="26" dataDxfId="78"/>
-    <tableColumn id="27" xr3:uid="{C835AA13-22A2-47F6-90DD-FCDCA26C8533}" uniqueName="27" name="T.Paid" queryTableFieldId="27" dataDxfId="77"/>
-    <tableColumn id="28" xr3:uid="{D5B33536-2DA2-4EF5-A4CA-CBC86952FCFD}" uniqueName="28" name="T.Balance" queryTableFieldId="28" dataDxfId="76"/>
-    <tableColumn id="29" xr3:uid="{7540773F-7F38-48F8-A327-608CAA69C844}" uniqueName="29" name="T.Payment" queryTableFieldId="29" dataDxfId="75"/>
-    <tableColumn id="30" xr3:uid="{00A2BD33-D24B-4919-A6A3-1B1243FE5D43}" uniqueName="30" name="T.IsPOS" queryTableFieldId="30" dataDxfId="74"/>
-    <tableColumn id="31" xr3:uid="{0A96AD8E-A700-4E3B-B9ED-BB0E47C0CB17}" uniqueName="31" name="T.IsRefund" queryTableFieldId="31" dataDxfId="73"/>
-    <tableColumn id="32" xr3:uid="{E46BAD2C-61CB-4939-BFA1-F053F3F0BF43}" uniqueName="32" name="T.IsCashSale" queryTableFieldId="32" dataDxfId="72"/>
-    <tableColumn id="33" xr3:uid="{490C93F1-2576-482D-AEF2-86D296A97DEC}" uniqueName="33" name="T.IsInvoice" queryTableFieldId="33" dataDxfId="71"/>
-    <tableColumn id="34" xr3:uid="{77956C28-A01C-4523-91E1-E090410C7531}" uniqueName="34" name="T.IsQuote" queryTableFieldId="34" dataDxfId="70"/>
-    <tableColumn id="35" xr3:uid="{BEA0A656-2014-4CBF-9858-C4B824336CE5}" uniqueName="35" name="T.IsSalesOrder" queryTableFieldId="35" dataDxfId="69"/>
-    <tableColumn id="36" xr3:uid="{9D4BC478-4145-44AA-9313-9A0498E4A145}" uniqueName="36" name="T.IsVoucher" queryTableFieldId="36" dataDxfId="68"/>
-    <tableColumn id="37" xr3:uid="{5D6AC46C-6670-46A6-A686-12E7267BD108}" uniqueName="37" name="T.IsLayby" queryTableFieldId="37" dataDxfId="67"/>
-    <tableColumn id="38" xr3:uid="{970224C3-C419-4100-AD4D-7D0DCE97235B}" uniqueName="38" name="T.IsLaybyTOS" queryTableFieldId="38" dataDxfId="66"/>
-    <tableColumn id="39" xr3:uid="{06FB0164-8C51-41B4-92E5-A00C159FF640}" uniqueName="39" name="T.IsLaybyPayment" queryTableFieldId="39" dataDxfId="65"/>
-    <tableColumn id="40" xr3:uid="{4CE0EE08-D1EE-416A-9558-B84BDEE52850}" uniqueName="40" name="T.IsCustomerReturn" queryTableFieldId="40" dataDxfId="64"/>
-    <tableColumn id="41" xr3:uid="{1173AAD9-4FCC-4C76-8295-65E7D8220CBF}" uniqueName="41" name="T.HoldSale" queryTableFieldId="41" dataDxfId="63"/>
-    <tableColumn id="42" xr3:uid="{3542BF0E-CB2B-40CF-AFEA-1DDF7549145D}" uniqueName="42" name="T.Converted" queryTableFieldId="42" dataDxfId="62"/>
-    <tableColumn id="43" xr3:uid="{D73B7502-DB22-4C63-81BB-019D698CAD59}" uniqueName="43" name="T.EnteredBy" queryTableFieldId="43" dataDxfId="61"/>
-    <tableColumn id="44" xr3:uid="{5539AAF4-02D6-4F2A-B8E9-4D2AB412A537}" uniqueName="44" name="T.QuoteStatus" queryTableFieldId="44" dataDxfId="60"/>
-    <tableColumn id="45" xr3:uid="{2EEA69F8-DF5C-4A1B-9C85-A50EF9221B0B}" uniqueName="45" name="T.ForeignExchangeCode" queryTableFieldId="45" dataDxfId="59"/>
-    <tableColumn id="46" xr3:uid="{8FD63CFF-5B87-4957-8383-0D162A66B5CE}" uniqueName="46" name="T.ForeignExchangeRate" queryTableFieldId="46" dataDxfId="58"/>
-    <tableColumn id="47" xr3:uid="{6B59FA58-121F-4D25-8646-CD655D303469}" uniqueName="47" name="T.ForeignTotalAmount" queryTableFieldId="47" dataDxfId="57"/>
-    <tableColumn id="48" xr3:uid="{53524585-07AD-4A87-B6CF-338992421B7F}" uniqueName="48" name="T.ForeignPaidAmount" queryTableFieldId="48" dataDxfId="56"/>
-    <tableColumn id="49" xr3:uid="{35ADF121-C9CB-4454-8876-2B377FEBCD3E}" uniqueName="49" name="T.ForeignBalanceAmount" queryTableFieldId="49" dataDxfId="55"/>
-    <tableColumn id="50" xr3:uid="{51EBD2CD-F1C7-4CA8-A6D2-062D87AEFA3D}" uniqueName="50" name="T.IsInternalOrder" queryTableFieldId="50" dataDxfId="54"/>
-    <tableColumn id="51" xr3:uid="{D760CAC5-115F-4DDE-904A-AEC728988090}" uniqueName="51" name="T.ContactName" queryTableFieldId="51" dataDxfId="53"/>
-    <tableColumn id="52" xr3:uid="{BE6E4943-BDB5-428A-A0FD-38871CA6C849}" uniqueName="52" name="T.Medtype" queryTableFieldId="52" dataDxfId="52"/>
-    <tableColumn id="53" xr3:uid="{ECE90855-0EB6-4905-834F-00631A702CFD}" uniqueName="53" name="T.SalesCategory" queryTableFieldId="53" dataDxfId="51"/>
-    <tableColumn id="54" xr3:uid="{EE2DECDE-C602-4F51-B666-2EC79F38ABAF}" uniqueName="54" name="T.SaleCustField1" queryTableFieldId="54" dataDxfId="50"/>
-    <tableColumn id="55" xr3:uid="{87DBF14C-605A-440E-AFEF-2513FDEE55A6}" uniqueName="55" name="T.SaleCustField2" queryTableFieldId="55" dataDxfId="49"/>
-    <tableColumn id="56" xr3:uid="{C55E6299-EA33-439B-A781-6FA45BCAAA66}" uniqueName="56" name="T.SaleCustField3" queryTableFieldId="56" dataDxfId="48"/>
-    <tableColumn id="57" xr3:uid="{13058FA4-9BDE-4CCF-A995-D63003ECC1FC}" uniqueName="57" name="T.SaleCustField4" queryTableFieldId="57" dataDxfId="47"/>
-    <tableColumn id="58" xr3:uid="{D0F66F2B-5A27-44DD-BF7B-A70DF9CDE4C7}" uniqueName="58" name="T.SaleCustField5" queryTableFieldId="58" dataDxfId="46"/>
-    <tableColumn id="59" xr3:uid="{9194B2F2-FC48-4AB9-8DF8-316C7722B890}" uniqueName="59" name="T.SaleCustField6" queryTableFieldId="59" dataDxfId="45"/>
-    <tableColumn id="60" xr3:uid="{965072AC-48E2-4BE1-98E3-26AB956823B1}" uniqueName="60" name="T.SaleCustField7" queryTableFieldId="60" dataDxfId="44"/>
-    <tableColumn id="61" xr3:uid="{82BD8DC3-AC79-4611-9CF0-858AFC7EF36B}" uniqueName="61" name="T.SaleCustField8" queryTableFieldId="61" dataDxfId="43"/>
-    <tableColumn id="62" xr3:uid="{3A873039-3566-4B0D-AB0F-F1EC4B83B0D8}" uniqueName="62" name="T.SaleCustField9" queryTableFieldId="62" dataDxfId="42"/>
-    <tableColumn id="63" xr3:uid="{22DA7826-9052-4D9B-9AF2-06C34526F6E9}" uniqueName="63" name="T.SaleCustField10" queryTableFieldId="63" dataDxfId="41"/>
-    <tableColumn id="64" xr3:uid="{3C10E8A5-223C-4EDF-90CD-9C1863163170}" uniqueName="64" name="T.AppointID" queryTableFieldId="64" dataDxfId="40"/>
-    <tableColumn id="65" xr3:uid="{70002DE5-E90B-4A34-BCF3-4FCA48B59ABF}" uniqueName="65" name="T.ReferenceNo" queryTableFieldId="65" dataDxfId="39"/>
-    <tableColumn id="66" xr3:uid="{690B69FC-E0CE-40EF-B0CC-D90E8A6EBC90}" uniqueName="66" name="T.SaleLineID" queryTableFieldId="66" dataDxfId="38"/>
-    <tableColumn id="67" xr3:uid="{2C0D6DFD-6738-41CE-9BBD-94E06D198231}" uniqueName="67" name="T.PARTTYPE" queryTableFieldId="67" dataDxfId="37"/>
-    <tableColumn id="68" xr3:uid="{C62B3477-988E-4298-8D55-87A3E97FF4F1}" uniqueName="68" name="T.INCOMEACCNT" queryTableFieldId="68" dataDxfId="36"/>
-    <tableColumn id="69" xr3:uid="{2084FBF9-AC8D-46D1-87BC-A3FD14E4366F}" uniqueName="69" name="T.ASSETACCNT" queryTableFieldId="69" dataDxfId="35"/>
-    <tableColumn id="70" xr3:uid="{33D7B053-EB79-401F-A3DE-59D40171E3F6}" uniqueName="70" name="T.COGSACCNT" queryTableFieldId="70" dataDxfId="34"/>
-    <tableColumn id="71" xr3:uid="{D57E48A7-C2C7-4231-A2E8-ABE9A8EC9637}" uniqueName="71" name="T.ProductName" queryTableFieldId="71" dataDxfId="33"/>
-    <tableColumn id="72" xr3:uid="{89766C40-066F-4EC8-8D02-D84617778EFC}" uniqueName="72" name="T.Product_Description" queryTableFieldId="72" dataDxfId="32"/>
-    <tableColumn id="73" xr3:uid="{FC3DEBD4-49C1-486F-B8AA-F867936ECBEB}" uniqueName="73" name="T.Product_Description_Memo" queryTableFieldId="73" dataDxfId="31"/>
-    <tableColumn id="74" xr3:uid="{E01A1F7A-411F-46A8-A7C2-A6E56C53E084}" uniqueName="74" name="T.LinePrice" queryTableFieldId="74" dataDxfId="30"/>
-    <tableColumn id="75" xr3:uid="{C3D7D106-3AB6-438D-A4DF-9BF16BF47E8B}" uniqueName="75" name="T.LinePriceInc" queryTableFieldId="75" dataDxfId="29"/>
-    <tableColumn id="76" xr3:uid="{A67412DD-1BB4-42B9-8B8A-461522FBDC2C}" uniqueName="76" name="T.LineTaxRate" queryTableFieldId="76" dataDxfId="28"/>
-    <tableColumn id="77" xr3:uid="{C48A1414-3FBF-4831-8370-ED06DC7DCA65}" uniqueName="77" name="T.LineCost" queryTableFieldId="77" dataDxfId="27"/>
-    <tableColumn id="78" xr3:uid="{823199A8-C387-418E-9FC0-D16DC9400C27}" uniqueName="78" name="T.LineCostInc" queryTableFieldId="78" dataDxfId="26"/>
-    <tableColumn id="79" xr3:uid="{596D9B29-18B0-41C1-B9F6-E4842246B1D4}" uniqueName="79" name="T.LineTaxCode" queryTableFieldId="79" dataDxfId="25"/>
-    <tableColumn id="80" xr3:uid="{BDCE9C8B-1C2B-4DC9-9231-EB7F7E751857}" uniqueName="80" name="T.LineTax" queryTableFieldId="80" dataDxfId="24"/>
-    <tableColumn id="81" xr3:uid="{64D80A30-7D4B-4811-8A25-8ADDCFB2B1BB}" uniqueName="81" name="T.QtySold" queryTableFieldId="81" dataDxfId="23"/>
-    <tableColumn id="82" xr3:uid="{784F40BA-F0F4-498B-986D-EA5218733403}" uniqueName="82" name="T.UnitofMeasureQtySold" queryTableFieldId="82" dataDxfId="22"/>
-    <tableColumn id="83" xr3:uid="{D1E03BF7-3484-4A1E-AC2A-296CDCE8100B}" uniqueName="83" name="T.Shipped" queryTableFieldId="83" dataDxfId="21"/>
-    <tableColumn id="84" xr3:uid="{6A365AF6-9000-41B1-A1C7-5800E7BC6B54}" uniqueName="84" name="T.UnitofMeasureShipped" queryTableFieldId="84" dataDxfId="20"/>
-    <tableColumn id="85" xr3:uid="{2E127C1A-D5DB-48E1-A091-B5BD96AD2D11}" uniqueName="85" name="T.BackOrder" queryTableFieldId="85" dataDxfId="19"/>
-    <tableColumn id="86" xr3:uid="{CACCE876-C703-46C4-A30F-CD327A2B04B8}" uniqueName="86" name="T.UnitofMeasureBackorder" queryTableFieldId="86" dataDxfId="18"/>
-    <tableColumn id="87" xr3:uid="{EEA6E02A-F3AA-4978-9142-7F37D3ABF081}" uniqueName="87" name="T.UnitofMeasureSaleLines" queryTableFieldId="87" dataDxfId="17"/>
-    <tableColumn id="88" xr3:uid="{128615A0-0644-4292-AE5D-DB19537674C3}" uniqueName="88" name="T.UnitofMeasureMultiplier" queryTableFieldId="88" dataDxfId="16"/>
-    <tableColumn id="89" xr3:uid="{B94E2350-D491-4EFD-8A16-9F9B63C22BF1}" uniqueName="89" name="T.Invoiced" queryTableFieldId="89" dataDxfId="15"/>
-    <tableColumn id="90" xr3:uid="{0DBA3E42-B354-487D-96CB-81D724445EA6}" uniqueName="90" name="T.Discounts" queryTableFieldId="90" dataDxfId="14"/>
-    <tableColumn id="91" xr3:uid="{3DD82A57-9AF2-487C-8215-F689B66546E5}" uniqueName="91" name="T.Markup" queryTableFieldId="91" dataDxfId="13"/>
-    <tableColumn id="92" xr3:uid="{C229DA29-0B68-4A36-AFBC-77246EA0FEFF}" uniqueName="92" name="T.Margin" queryTableFieldId="92" dataDxfId="12"/>
-    <tableColumn id="93" xr3:uid="{9EA61FDA-659C-4BE8-B709-388F34AC66EC}" uniqueName="93" name="T.MarkupPercent" queryTableFieldId="93" dataDxfId="11"/>
-    <tableColumn id="94" xr3:uid="{5FDBA985-260B-41B1-864D-107705517B7A}" uniqueName="94" name="T.DiscountPercent" queryTableFieldId="94" dataDxfId="10"/>
-    <tableColumn id="95" xr3:uid="{84951EFF-C289-46B5-806A-187913777D2E}" uniqueName="95" name="T.MarginPercent" queryTableFieldId="95" dataDxfId="9"/>
-    <tableColumn id="96" xr3:uid="{D0CA2843-418C-43E2-8C6C-DC936B7AC8AE}" uniqueName="96" name="T.TotalLineAmount" queryTableFieldId="96" dataDxfId="8"/>
-    <tableColumn id="97" xr3:uid="{77013A01-1BD5-4C5F-A70B-0865D5675DFE}" uniqueName="97" name="T.TotalLineAmountInc" queryTableFieldId="97" dataDxfId="7"/>
-    <tableColumn id="98" xr3:uid="{8272C50B-2A8C-4D4D-812C-DF13F6972910}" uniqueName="98" name="T.RefundQty" queryTableFieldId="98" dataDxfId="6"/>
-    <tableColumn id="99" xr3:uid="{811B8C81-0E63-4C2F-95ED-632CA546698E}" uniqueName="99" name="T.ForeignCurrencyLinePrice" queryTableFieldId="99" dataDxfId="5"/>
-    <tableColumn id="100" xr3:uid="{56D45762-E995-415C-AF87-8FCD1E4CD6A2}" uniqueName="100" name="T.ForeignTotalLineAmount" queryTableFieldId="100" dataDxfId="4"/>
-    <tableColumn id="101" xr3:uid="{0124CB98-DB3A-4697-AF0D-B23A88D20E40}" uniqueName="101" name="T.ShipDate_1" queryTableFieldId="101" dataDxfId="3"/>
-    <tableColumn id="102" xr3:uid="{58FFE36C-2DC5-4F8D-BCB4-21DC8C2FFBAA}" uniqueName="102" name="T.ETDDate" queryTableFieldId="102" dataDxfId="2"/>
-    <tableColumn id="103" xr3:uid="{107CAE8D-9422-4E19-B220-3F1777D0F5A4}" uniqueName="103" name="T.ReferenceNo_1" queryTableFieldId="103" dataDxfId="1"/>
-    <tableColumn id="104" xr3:uid="{F352AD05-B95F-4D38-8D0F-3A0835F24AB2}" uniqueName="104" name="T.SaleID" queryTableFieldId="104" dataDxfId="0"/>
+    <tableColumn id="105" uniqueName="105" name="T.InvoiceDocNumber" queryTableFieldId="1" dataDxfId="103"/>
+    <tableColumn id="2" uniqueName="2" name="T.Account" queryTableFieldId="2" dataDxfId="102"/>
+    <tableColumn id="3" uniqueName="3" name="T.CustomerName" queryTableFieldId="3" dataDxfId="101"/>
+    <tableColumn id="4" uniqueName="4" name="T.InvoiceTo" queryTableFieldId="4" dataDxfId="100"/>
+    <tableColumn id="5" uniqueName="5" name="T.ShipTo" queryTableFieldId="5" dataDxfId="99"/>
+    <tableColumn id="6" uniqueName="6" name="T.PickupFrom" queryTableFieldId="6" dataDxfId="98"/>
+    <tableColumn id="7" uniqueName="7" name="T.SaleDate" queryTableFieldId="7" dataDxfId="97"/>
+    <tableColumn id="8" uniqueName="8" name="T.TotalTax" queryTableFieldId="8" dataDxfId="96"/>
+    <tableColumn id="9" uniqueName="9" name="T.TotalAmount" queryTableFieldId="9" dataDxfId="95"/>
+    <tableColumn id="10" uniqueName="10" name="T.TotalAmountInc" queryTableFieldId="10" dataDxfId="94"/>
+    <tableColumn id="11" uniqueName="11" name="T.TotalMarkup" queryTableFieldId="11" dataDxfId="93"/>
+    <tableColumn id="12" uniqueName="12" name="T.TotalDiscount" queryTableFieldId="12" dataDxfId="92"/>
+    <tableColumn id="13" uniqueName="13" name="T.EmployeeName" queryTableFieldId="13" dataDxfId="91"/>
+    <tableColumn id="14" uniqueName="14" name="T.Class" queryTableFieldId="14" dataDxfId="90"/>
+    <tableColumn id="15" uniqueName="15" name="T.OrderNumber" queryTableFieldId="15" dataDxfId="89"/>
+    <tableColumn id="16" uniqueName="16" name="T.PONumber" queryTableFieldId="16" dataDxfId="88"/>
+    <tableColumn id="17" uniqueName="17" name="T.ChequeNo" queryTableFieldId="17" dataDxfId="87"/>
+    <tableColumn id="18" uniqueName="18" name="T.ShipDate" queryTableFieldId="18" dataDxfId="86"/>
+    <tableColumn id="19" uniqueName="19" name="T.FutureSO" queryTableFieldId="19" dataDxfId="85"/>
+    <tableColumn id="20" uniqueName="20" name="T.DueDate" queryTableFieldId="20" dataDxfId="84"/>
+    <tableColumn id="21" uniqueName="21" name="T.ConNote" queryTableFieldId="21" dataDxfId="83"/>
+    <tableColumn id="22" uniqueName="22" name="T.Comments" queryTableFieldId="22" dataDxfId="82"/>
+    <tableColumn id="23" uniqueName="23" name="T.Shipping" queryTableFieldId="23" dataDxfId="81"/>
+    <tableColumn id="24" uniqueName="24" name="T.Terms" queryTableFieldId="24" dataDxfId="80"/>
+    <tableColumn id="25" uniqueName="25" name="T.PayMethod" queryTableFieldId="25" dataDxfId="79"/>
+    <tableColumn id="26" uniqueName="26" name="T.PayDueDate" queryTableFieldId="26" dataDxfId="78"/>
+    <tableColumn id="27" uniqueName="27" name="T.Paid" queryTableFieldId="27" dataDxfId="77"/>
+    <tableColumn id="28" uniqueName="28" name="T.Balance" queryTableFieldId="28" dataDxfId="76"/>
+    <tableColumn id="29" uniqueName="29" name="T.Payment" queryTableFieldId="29" dataDxfId="75"/>
+    <tableColumn id="30" uniqueName="30" name="T.IsPOS" queryTableFieldId="30" dataDxfId="74"/>
+    <tableColumn id="31" uniqueName="31" name="T.IsRefund" queryTableFieldId="31" dataDxfId="73"/>
+    <tableColumn id="32" uniqueName="32" name="T.IsCashSale" queryTableFieldId="32" dataDxfId="72"/>
+    <tableColumn id="33" uniqueName="33" name="T.IsInvoice" queryTableFieldId="33" dataDxfId="71"/>
+    <tableColumn id="34" uniqueName="34" name="T.IsQuote" queryTableFieldId="34" dataDxfId="70"/>
+    <tableColumn id="35" uniqueName="35" name="T.IsSalesOrder" queryTableFieldId="35" dataDxfId="69"/>
+    <tableColumn id="36" uniqueName="36" name="T.IsVoucher" queryTableFieldId="36" dataDxfId="68"/>
+    <tableColumn id="37" uniqueName="37" name="T.IsLayby" queryTableFieldId="37" dataDxfId="67"/>
+    <tableColumn id="38" uniqueName="38" name="T.IsLaybyTOS" queryTableFieldId="38" dataDxfId="66"/>
+    <tableColumn id="39" uniqueName="39" name="T.IsLaybyPayment" queryTableFieldId="39" dataDxfId="65"/>
+    <tableColumn id="40" uniqueName="40" name="T.IsCustomerReturn" queryTableFieldId="40" dataDxfId="64"/>
+    <tableColumn id="41" uniqueName="41" name="T.HoldSale" queryTableFieldId="41" dataDxfId="63"/>
+    <tableColumn id="42" uniqueName="42" name="T.Converted" queryTableFieldId="42" dataDxfId="62"/>
+    <tableColumn id="43" uniqueName="43" name="T.EnteredBy" queryTableFieldId="43" dataDxfId="61"/>
+    <tableColumn id="44" uniqueName="44" name="T.QuoteStatus" queryTableFieldId="44" dataDxfId="60"/>
+    <tableColumn id="45" uniqueName="45" name="T.ForeignExchangeCode" queryTableFieldId="45" dataDxfId="59"/>
+    <tableColumn id="46" uniqueName="46" name="T.ForeignExchangeRate" queryTableFieldId="46" dataDxfId="58"/>
+    <tableColumn id="47" uniqueName="47" name="T.ForeignTotalAmount" queryTableFieldId="47" dataDxfId="57"/>
+    <tableColumn id="48" uniqueName="48" name="T.ForeignPaidAmount" queryTableFieldId="48" dataDxfId="56"/>
+    <tableColumn id="49" uniqueName="49" name="T.ForeignBalanceAmount" queryTableFieldId="49" dataDxfId="55"/>
+    <tableColumn id="50" uniqueName="50" name="T.IsInternalOrder" queryTableFieldId="50" dataDxfId="54"/>
+    <tableColumn id="51" uniqueName="51" name="T.ContactName" queryTableFieldId="51" dataDxfId="53"/>
+    <tableColumn id="52" uniqueName="52" name="T.Medtype" queryTableFieldId="52" dataDxfId="52"/>
+    <tableColumn id="53" uniqueName="53" name="T.SalesCategory" queryTableFieldId="53" dataDxfId="51"/>
+    <tableColumn id="54" uniqueName="54" name="T.SaleCustField1" queryTableFieldId="54" dataDxfId="50"/>
+    <tableColumn id="55" uniqueName="55" name="T.SaleCustField2" queryTableFieldId="55" dataDxfId="49"/>
+    <tableColumn id="56" uniqueName="56" name="T.SaleCustField3" queryTableFieldId="56" dataDxfId="48"/>
+    <tableColumn id="57" uniqueName="57" name="T.SaleCustField4" queryTableFieldId="57" dataDxfId="47"/>
+    <tableColumn id="58" uniqueName="58" name="T.SaleCustField5" queryTableFieldId="58" dataDxfId="46"/>
+    <tableColumn id="59" uniqueName="59" name="T.SaleCustField6" queryTableFieldId="59" dataDxfId="45"/>
+    <tableColumn id="60" uniqueName="60" name="T.SaleCustField7" queryTableFieldId="60" dataDxfId="44"/>
+    <tableColumn id="61" uniqueName="61" name="T.SaleCustField8" queryTableFieldId="61" dataDxfId="43"/>
+    <tableColumn id="62" uniqueName="62" name="T.SaleCustField9" queryTableFieldId="62" dataDxfId="42"/>
+    <tableColumn id="63" uniqueName="63" name="T.SaleCustField10" queryTableFieldId="63" dataDxfId="41"/>
+    <tableColumn id="64" uniqueName="64" name="T.AppointID" queryTableFieldId="64" dataDxfId="40"/>
+    <tableColumn id="65" uniqueName="65" name="T.ReferenceNo" queryTableFieldId="65" dataDxfId="39"/>
+    <tableColumn id="66" uniqueName="66" name="T.SaleLineID" queryTableFieldId="66" dataDxfId="38"/>
+    <tableColumn id="67" uniqueName="67" name="T.PARTTYPE" queryTableFieldId="67" dataDxfId="37"/>
+    <tableColumn id="68" uniqueName="68" name="T.INCOMEACCNT" queryTableFieldId="68" dataDxfId="36"/>
+    <tableColumn id="69" uniqueName="69" name="T.ASSETACCNT" queryTableFieldId="69" dataDxfId="35"/>
+    <tableColumn id="70" uniqueName="70" name="T.COGSACCNT" queryTableFieldId="70" dataDxfId="34"/>
+    <tableColumn id="71" uniqueName="71" name="T.ProductName" queryTableFieldId="71" dataDxfId="33"/>
+    <tableColumn id="72" uniqueName="72" name="T.Product_Description" queryTableFieldId="72" dataDxfId="32"/>
+    <tableColumn id="73" uniqueName="73" name="T.Product_Description_Memo" queryTableFieldId="73" dataDxfId="31"/>
+    <tableColumn id="74" uniqueName="74" name="T.LinePrice" queryTableFieldId="74" dataDxfId="30"/>
+    <tableColumn id="75" uniqueName="75" name="T.LinePriceInc" queryTableFieldId="75" dataDxfId="29"/>
+    <tableColumn id="76" uniqueName="76" name="T.LineTaxRate" queryTableFieldId="76" dataDxfId="28"/>
+    <tableColumn id="77" uniqueName="77" name="T.LineCost" queryTableFieldId="77" dataDxfId="27"/>
+    <tableColumn id="78" uniqueName="78" name="T.LineCostInc" queryTableFieldId="78" dataDxfId="26"/>
+    <tableColumn id="79" uniqueName="79" name="T.LineTaxCode" queryTableFieldId="79" dataDxfId="25"/>
+    <tableColumn id="80" uniqueName="80" name="T.LineTax" queryTableFieldId="80" dataDxfId="24"/>
+    <tableColumn id="81" uniqueName="81" name="T.QtySold" queryTableFieldId="81" dataDxfId="23"/>
+    <tableColumn id="82" uniqueName="82" name="T.UnitofMeasureQtySold" queryTableFieldId="82" dataDxfId="22"/>
+    <tableColumn id="83" uniqueName="83" name="T.Shipped" queryTableFieldId="83" dataDxfId="21"/>
+    <tableColumn id="84" uniqueName="84" name="T.UnitofMeasureShipped" queryTableFieldId="84" dataDxfId="20"/>
+    <tableColumn id="85" uniqueName="85" name="T.BackOrder" queryTableFieldId="85" dataDxfId="19"/>
+    <tableColumn id="86" uniqueName="86" name="T.UnitofMeasureBackorder" queryTableFieldId="86" dataDxfId="18"/>
+    <tableColumn id="87" uniqueName="87" name="T.UnitofMeasureSaleLines" queryTableFieldId="87" dataDxfId="17"/>
+    <tableColumn id="88" uniqueName="88" name="T.UnitofMeasureMultiplier" queryTableFieldId="88" dataDxfId="16"/>
+    <tableColumn id="89" uniqueName="89" name="T.Invoiced" queryTableFieldId="89" dataDxfId="15"/>
+    <tableColumn id="90" uniqueName="90" name="T.Discounts" queryTableFieldId="90" dataDxfId="14"/>
+    <tableColumn id="91" uniqueName="91" name="T.Markup" queryTableFieldId="91" dataDxfId="13"/>
+    <tableColumn id="92" uniqueName="92" name="T.Margin" queryTableFieldId="92" dataDxfId="12"/>
+    <tableColumn id="93" uniqueName="93" name="T.MarkupPercent" queryTableFieldId="93" dataDxfId="11"/>
+    <tableColumn id="94" uniqueName="94" name="T.DiscountPercent" queryTableFieldId="94" dataDxfId="10"/>
+    <tableColumn id="95" uniqueName="95" name="T.MarginPercent" queryTableFieldId="95" dataDxfId="9"/>
+    <tableColumn id="96" uniqueName="96" name="T.TotalLineAmount" queryTableFieldId="96" dataDxfId="8"/>
+    <tableColumn id="97" uniqueName="97" name="T.TotalLineAmountInc" queryTableFieldId="97" dataDxfId="7"/>
+    <tableColumn id="98" uniqueName="98" name="T.RefundQty" queryTableFieldId="98" dataDxfId="6"/>
+    <tableColumn id="99" uniqueName="99" name="T.ForeignCurrencyLinePrice" queryTableFieldId="99" dataDxfId="5"/>
+    <tableColumn id="100" uniqueName="100" name="T.ForeignTotalLineAmount" queryTableFieldId="100" dataDxfId="4"/>
+    <tableColumn id="101" uniqueName="101" name="T.ShipDate_1" queryTableFieldId="101" dataDxfId="3"/>
+    <tableColumn id="102" uniqueName="102" name="T.ETDDate" queryTableFieldId="102" dataDxfId="2"/>
+    <tableColumn id="103" uniqueName="103" name="T.ReferenceNo_1" queryTableFieldId="103" dataDxfId="1"/>
+    <tableColumn id="104" uniqueName="104" name="T.SaleID" queryTableFieldId="104" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2876,30 +2830,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.25" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="29.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>236</v>
       </c>
@@ -2924,7 +2880,7 @@
       <c r="H1" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>244</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -2933,798 +2889,1332 @@
       <c r="K1" s="2" t="s">
         <v>246</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="2" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="str">
+        <f>'Raw Data'!$G$2</f>
         <v>2023-01-13 00:00:00</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>1050</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B2" s="4">
+        <f>'Raw Data'!$BN$2</f>
+        <v>1970</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>'Raw Data'!$T$2</f>
         <v>2023-01-27 00:00:00</v>
       </c>
-      <c r="D2" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D2" s="4" t="str">
+        <f>'Raw Data'!$C$2</f>
         <v>Wang Song</v>
       </c>
-      <c r="E2" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E2" s="4" t="str">
+        <f>'Raw Data'!$BS$2</f>
         <v>aaa</v>
       </c>
-      <c r="F2" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F2" s="4" t="str">
+        <f>'Raw Data'!$BT$2</f>
         <v/>
       </c>
-      <c r="G2" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I2" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G2" s="4" t="str">
+        <f>'Raw Data'!$CX$2</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H2" s="4" t="str">
+        <f>'Raw Data'!$BQ$2</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I2" s="5">
+        <f>'Raw Data'!$CC$2</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="str">
+        <f>'Raw Data'!$AR$2</f>
         <v/>
       </c>
+      <c r="K2" s="4" t="str">
+        <f>'Raw Data'!$V$2</f>
+        <v/>
+      </c>
+      <c r="L2" s="4" t="str">
+        <f>'Raw Data'!$R$2</f>
+        <v>2023-01-13 00:00:00</v>
+      </c>
+      <c r="M2" s="4" t="str">
+        <f>'Raw Data'!$AQ$2</f>
+        <v>Dene User</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="3" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5">
+        <f>SUBTOTAL(9,I2:I2)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="str">
+        <f>'Raw Data'!$G$3</f>
         <v>2022-12-19 00:00:00</v>
       </c>
-      <c r="B3" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>983</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B4" s="4">
+        <f>'Raw Data'!$BN$3</f>
+        <v>1852</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <f>'Raw Data'!$T$3</f>
         <v>2022-12-26 00:00:00</v>
       </c>
-      <c r="D3" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D4" s="4" t="str">
+        <f>'Raw Data'!C3</f>
         <v>ABC Company</v>
       </c>
-      <c r="E3" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E4" s="4" t="str">
+        <f>'Raw Data'!$BS$3</f>
         <v>10 Unit</v>
       </c>
-      <c r="F3" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F4" s="4" t="str">
+        <f>'Raw Data'!$BT$3</f>
         <v>- For unit currency</v>
       </c>
-      <c r="G3" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I3" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G4" s="4" t="str">
+        <f>'Raw Data'!$CX$3</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H4" s="4" t="str">
+        <f>'Raw Data'!$BQ$3</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I4" s="5">
+        <f>'Raw Data'!$CC$3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>9.0909099999999992</v>
-      </c>
-      <c r="K3" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J4" s="4" t="str">
+        <f>'Raw Data'!$AR$3</f>
         <v/>
       </c>
+      <c r="K4" s="4" t="str">
+        <f>'Raw Data'!$V$3</f>
+        <v/>
+      </c>
+      <c r="L4" s="4" t="str">
+        <f>'Raw Data'!$R$3</f>
+        <v>2022-12-19 00:00:00</v>
+      </c>
+      <c r="M4" s="4" t="str">
+        <f>'Raw Data'!$AQ$3</f>
+        <v>Dene User</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="5" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5">
+        <f>SUBTOTAL(9,I4:I4)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="str">
+        <f>'Raw Data'!$G$4</f>
         <v>2022-06-29 00:00:00</v>
       </c>
-      <c r="B4" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>825</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B6" s="4">
+        <f>'Raw Data'!$BN$4</f>
+        <v>1711</v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <f>'Raw Data'!$T$4</f>
         <v>2022-07-06 00:00:00</v>
       </c>
-      <c r="D4" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D6" s="4" t="str">
+        <f>'Raw Data'!C4</f>
         <v>Wang Song</v>
       </c>
-      <c r="E4" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E6" s="4" t="str">
+        <f>'Raw Data'!$BS$4</f>
         <v>Fanta Orange Can</v>
       </c>
-      <c r="F4" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F6" s="4" t="str">
+        <f>'Raw Data'!$BT$4</f>
         <v xml:space="preserve">
                                         Fanta Orange Can Soda</v>
       </c>
-      <c r="G4" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I4" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G6" s="4" t="str">
+        <f>'Raw Data'!$CX$4</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H6" s="4" t="str">
+        <f>'Raw Data'!$BQ$4</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I6" s="5">
+        <f>'Raw Data'!$CC$4</f>
         <v>1</v>
       </c>
-      <c r="J4" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>6</v>
-      </c>
-      <c r="K4" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J6" s="4" t="str">
+        <f>'Raw Data'!$AR$4</f>
         <v>Invoiced</v>
       </c>
+      <c r="K6" s="4" t="str">
+        <f>'Raw Data'!$V$4</f>
+        <v>This is testing</v>
+      </c>
+      <c r="L6" s="4" t="str">
+        <f>'Raw Data'!$R$4</f>
+        <v>2022-06-29 00:00:00</v>
+      </c>
+      <c r="M6" s="4" t="str">
+        <f>'Raw Data'!$AQ$4</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="7" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5">
+        <f>SUBTOTAL(9,I6:I6)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="str">
+        <f>'Raw Data'!$G$5</f>
         <v>2022-03-30 00:00:00</v>
       </c>
-      <c r="B5" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>730</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B8" s="4">
+        <f>'Raw Data'!$BN$5</f>
+        <v>1448</v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <f>'Raw Data'!$T$5</f>
         <v>2022-04-06 00:00:00</v>
       </c>
-      <c r="D5" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D8" s="4" t="str">
+        <f>'Raw Data'!C5</f>
         <v>Car Wash Express</v>
       </c>
-      <c r="E5" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E8" s="4" t="str">
+        <f>'Raw Data'!$BS$5</f>
         <v>Fanta Orange Can</v>
       </c>
-      <c r="F5" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F8" s="4" t="str">
+        <f>'Raw Data'!$BT$5</f>
         <v>Fanta Orange Can Soda</v>
       </c>
-      <c r="G5" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I5" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G8" s="4" t="str">
+        <f>'Raw Data'!$CX$5</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f>'Raw Data'!$BQ$5</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I8" s="5">
+        <f>'Raw Data'!$CC$5</f>
         <v>5</v>
       </c>
-      <c r="J5" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>6</v>
-      </c>
-      <c r="K5" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J8" s="4" t="str">
+        <f>'Raw Data'!$AR$5</f>
         <v/>
       </c>
+      <c r="K8" s="4" t="str">
+        <f>'Raw Data'!$V$5</f>
+        <v/>
+      </c>
+      <c r="L8" s="4" t="str">
+        <f>'Raw Data'!$R$5</f>
+        <v>2022-03-30 00:00:00</v>
+      </c>
+      <c r="M8" s="4" t="str">
+        <f>'Raw Data'!$AQ$5</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="9" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5">
+        <f>SUBTOTAL(9,I8:I8)</f>
+        <v>5</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="str">
+        <f>'Raw Data'!$G$6</f>
         <v>2021-12-07 00:00:00</v>
       </c>
-      <c r="B6" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>694</v>
-      </c>
-      <c r="C6" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B10" s="4">
+        <f>'Raw Data'!$BN$6</f>
+        <v>1407</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <f>'Raw Data'!$T$6</f>
         <v>2021-12-14 00:00:00</v>
       </c>
-      <c r="D6" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D10" s="4" t="str">
+        <f>'Raw Data'!C6</f>
         <v>ABC Company^Plumber</v>
       </c>
-      <c r="E6" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E10" s="4" t="str">
+        <f>'Raw Data'!$BS$6</f>
         <v>PC Mouse</v>
       </c>
-      <c r="F6" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F10" s="4" t="str">
+        <f>'Raw Data'!$BT$6</f>
         <v>PC Mouse Black</v>
       </c>
-      <c r="G6" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I6" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G10" s="4" t="str">
+        <f>'Raw Data'!$CX$6</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H10" s="4" t="str">
+        <f>'Raw Data'!$BQ$6</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I10" s="5">
+        <f>'Raw Data'!$CC$6</f>
         <v>18</v>
       </c>
-      <c r="J6" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>20</v>
-      </c>
-      <c r="K6" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J10" s="4" t="str">
+        <f>'Raw Data'!$AR$6</f>
         <v/>
       </c>
+      <c r="K10" s="4" t="str">
+        <f>'Raw Data'!$V$6</f>
+        <v/>
+      </c>
+      <c r="L10" s="4" t="str">
+        <f>'Raw Data'!$R$6</f>
+        <v>2021-12-07 00:00:00</v>
+      </c>
+      <c r="M10" s="4" t="str">
+        <f>'Raw Data'!$AQ$6</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="11" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="str">
+        <f>'Raw Data'!$G$7</f>
         <v>2021-12-07 00:00:00</v>
       </c>
-      <c r="B7" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>694</v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B11" s="4">
+        <f>'Raw Data'!$BN$7</f>
+        <v>1408</v>
+      </c>
+      <c r="C11" s="4" t="str">
+        <f>'Raw Data'!$T$7</f>
         <v>2021-12-14 00:00:00</v>
       </c>
-      <c r="D7" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D11" s="4" t="str">
+        <f>'Raw Data'!C7</f>
         <v>ABC Company^Plumber</v>
       </c>
-      <c r="E7" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E11" s="4" t="str">
+        <f>'Raw Data'!$BS$7</f>
         <v>PC Mouse</v>
       </c>
-      <c r="F7" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F11" s="4" t="str">
+        <f>'Raw Data'!$BT$7</f>
         <v>PC Mouse Black</v>
       </c>
-      <c r="G7" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I7" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G11" s="4" t="str">
+        <f>'Raw Data'!$CX$7</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H11" s="4" t="str">
+        <f>'Raw Data'!$BQ$7</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I11" s="5">
+        <f>'Raw Data'!$CC$7</f>
         <v>19</v>
       </c>
-      <c r="J7" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>20</v>
-      </c>
-      <c r="K7" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J11" s="4" t="str">
+        <f>'Raw Data'!$AR$7</f>
         <v/>
       </c>
+      <c r="K11" s="4" t="str">
+        <f>'Raw Data'!$V$7</f>
+        <v/>
+      </c>
+      <c r="L11" s="4" t="str">
+        <f>'Raw Data'!$R$7</f>
+        <v>2021-12-07 00:00:00</v>
+      </c>
+      <c r="M11" s="4" t="str">
+        <f>'Raw Data'!$AQ$7</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="12" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="5">
+        <f>SUBTOTAL(9,I10:I11)</f>
+        <v>37</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="str">
+        <f>'Raw Data'!$G$8</f>
         <v>2021-10-08 00:00:00</v>
       </c>
-      <c r="B8" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>361</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B13" s="4">
+        <f>'Raw Data'!$BN$8</f>
+        <v>1266</v>
+      </c>
+      <c r="C13" s="4" t="str">
+        <f>'Raw Data'!$T$8</f>
         <v>2021-10-08 00:00:00</v>
       </c>
-      <c r="D8" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D13" s="4" t="str">
+        <f>'Raw Data'!C8</f>
         <v>ABC</v>
       </c>
-      <c r="E8" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E13" s="4" t="str">
+        <f>'Raw Data'!$BS$8</f>
         <v>Keyboard</v>
       </c>
-      <c r="F8" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F13" s="4" t="str">
+        <f>'Raw Data'!$BT$8</f>
         <v>Keyboard Black</v>
       </c>
-      <c r="G8" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I8" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>10</v>
-      </c>
-      <c r="K8" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G13" s="4" t="str">
+        <f>'Raw Data'!$CX$8</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f>'Raw Data'!$BQ$8</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I13" s="5">
+        <f>'Raw Data'!$CC$8</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="4" t="str">
+        <f>'Raw Data'!$AR$8</f>
         <v/>
       </c>
+      <c r="K13" s="4" t="str">
+        <f>'Raw Data'!$V$8</f>
+        <v/>
+      </c>
+      <c r="L13" s="4" t="str">
+        <f>'Raw Data'!$R$8</f>
+        <v>2021-10-08 00:00:00</v>
+      </c>
+      <c r="M13" s="4" t="str">
+        <f>'Raw Data'!$AQ$8</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="14" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="str">
+        <f>'Raw Data'!$G$9</f>
         <v>2021-10-08 00:00:00</v>
       </c>
-      <c r="B9" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>361</v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B14" s="4">
+        <f>'Raw Data'!$BN$9</f>
+        <v>1267</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <f>'Raw Data'!$T$9</f>
         <v>2021-10-08 00:00:00</v>
       </c>
-      <c r="D9" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D14" s="4" t="str">
+        <f>'Raw Data'!C9</f>
         <v>ABC</v>
       </c>
-      <c r="E9" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E14" s="4" t="str">
+        <f>'Raw Data'!$BS$9</f>
         <v>PC Mouse</v>
       </c>
-      <c r="F9" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F14" s="4" t="str">
+        <f>'Raw Data'!$BT$9</f>
         <v>PC Mouse Black</v>
       </c>
-      <c r="G9" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I9" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>20</v>
-      </c>
-      <c r="K9" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G14" s="4" t="str">
+        <f>'Raw Data'!$CX$9</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H14" s="4" t="str">
+        <f>'Raw Data'!$BQ$9</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I14" s="5">
+        <f>'Raw Data'!$CC$9</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4" t="str">
+        <f>'Raw Data'!$AR$9</f>
         <v/>
       </c>
+      <c r="K14" s="4" t="str">
+        <f>'Raw Data'!$V$9</f>
+        <v/>
+      </c>
+      <c r="L14" s="4" t="str">
+        <f>'Raw Data'!$R$9</f>
+        <v>2021-10-08 00:00:00</v>
+      </c>
+      <c r="M14" s="4" t="str">
+        <f>'Raw Data'!$AQ$9</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="15" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="5">
+        <f>SUBTOTAL(9,I13:I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="str">
+        <f>'Raw Data'!$G$10</f>
         <v>2021-04-28 00:00:00</v>
       </c>
-      <c r="B10" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>354</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B16" s="4">
+        <f>'Raw Data'!$BN$10</f>
+        <v>739</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>'Raw Data'!$T$10</f>
         <v>2021-05-05 00:00:00</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D16" s="4" t="str">
+        <f>'Raw Data'!C10</f>
         <v>4X4 World^Constructions</v>
       </c>
-      <c r="E10" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E16" s="4" t="str">
+        <f>'Raw Data'!$BS$10</f>
         <v>500ml Red Wine</v>
       </c>
-      <c r="F10" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F16" s="4" t="str">
+        <f>'Raw Data'!$BT$10</f>
         <v>500ml Red Wine Van der Berg</v>
       </c>
-      <c r="G10" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I10" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G16" s="4" t="str">
+        <f>'Raw Data'!$CX$10</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H16" s="4" t="str">
+        <f>'Raw Data'!$BQ$10</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I16" s="5">
+        <f>'Raw Data'!$CC$10</f>
         <v>1</v>
       </c>
-      <c r="J10" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>16</v>
-      </c>
-      <c r="K10" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J16" s="4" t="str">
+        <f>'Raw Data'!$AR$10</f>
         <v/>
       </c>
+      <c r="K16" s="4" t="str">
+        <f>'Raw Data'!$V$10</f>
+        <v/>
+      </c>
+      <c r="L16" s="4" t="str">
+        <f>'Raw Data'!$R$10</f>
+        <v>2021-04-28 00:00:00</v>
+      </c>
+      <c r="M16" s="4" t="str">
+        <f>'Raw Data'!$AQ$10</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="17" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="5">
+        <f>SUBTOTAL(9,I16:I16)</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="str">
+        <f>'Raw Data'!$G$11</f>
         <v>2021-10-08 00:00:00</v>
       </c>
-      <c r="B11" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>345</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B18" s="4">
+        <f>'Raw Data'!$BN$11</f>
+        <v>742</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f>'Raw Data'!$T$11</f>
         <v>2021-10-22 00:00:00</v>
       </c>
-      <c r="D11" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D18" s="4" t="str">
+        <f>'Raw Data'!C11</f>
         <v>k c Sunshine^Job Test</v>
       </c>
-      <c r="E11" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E18" s="4" t="str">
+        <f>'Raw Data'!$BS$11</f>
         <v>Large Wagon</v>
       </c>
-      <c r="F11" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F18" s="4" t="str">
+        <f>'Raw Data'!$BT$11</f>
         <v>Large Wagon Red</v>
       </c>
-      <c r="G11" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I11" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G18" s="4" t="str">
+        <f>'Raw Data'!$CX$11</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H18" s="4" t="str">
+        <f>'Raw Data'!$BQ$11</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I18" s="5">
+        <f>'Raw Data'!$CC$11</f>
         <v>1</v>
       </c>
-      <c r="J11" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>800</v>
-      </c>
-      <c r="K11" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J18" s="4" t="str">
+        <f>'Raw Data'!$AR$11</f>
         <v>Approved</v>
       </c>
+      <c r="K18" s="4" t="str">
+        <f>'Raw Data'!$V$11</f>
+        <v/>
+      </c>
+      <c r="L18" s="4" t="str">
+        <f>'Raw Data'!$R$11</f>
+        <v>2021-10-08 00:00:00</v>
+      </c>
+      <c r="M18" s="4" t="str">
+        <f>'Raw Data'!$AQ$11</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="19" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5">
+        <f>SUBTOTAL(9,I18:I18)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="str">
+        <f>'Raw Data'!$G$12</f>
         <v>2021-01-13 00:00:00</v>
       </c>
-      <c r="B12" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>230</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B20" s="4">
+        <f>'Raw Data'!$BN$12</f>
+        <v>438</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f>'Raw Data'!$T$12</f>
         <v>2021-01-27 00:00:00</v>
       </c>
-      <c r="D12" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D20" s="4" t="str">
+        <f>'Raw Data'!C12</f>
         <v>4X4 World</v>
       </c>
-      <c r="E12" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E20" s="4" t="str">
+        <f>'Raw Data'!$BS$12</f>
         <v>Monitor 607</v>
       </c>
-      <c r="F12" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F20" s="4" t="str">
+        <f>'Raw Data'!$BT$12</f>
         <v>Asus Monitor 607</v>
       </c>
-      <c r="G12" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I12" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G20" s="4" t="str">
+        <f>'Raw Data'!$CX$12</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H20" s="4" t="str">
+        <f>'Raw Data'!$BQ$12</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I20" s="5">
+        <f>'Raw Data'!$CC$12</f>
         <v>1</v>
       </c>
-      <c r="J12" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>99</v>
-      </c>
-      <c r="K12" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J20" s="4" t="str">
+        <f>'Raw Data'!$AR$12</f>
         <v/>
       </c>
+      <c r="K20" s="4" t="str">
+        <f>'Raw Data'!$V$12</f>
+        <v/>
+      </c>
+      <c r="L20" s="4" t="str">
+        <f>'Raw Data'!$R$12</f>
+        <v>2021-01-13 00:00:00</v>
+      </c>
+      <c r="M20" s="4" t="str">
+        <f>'Raw Data'!$AQ$12</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="21" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="str">
+        <f>'Raw Data'!$G$13</f>
         <v>2021-01-13 00:00:00</v>
       </c>
-      <c r="B13" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>227</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B21" s="4">
+        <f>'Raw Data'!$BN$13</f>
+        <v>436</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f>'Raw Data'!$T$13</f>
         <v>2021-01-27 00:00:00</v>
       </c>
-      <c r="D13" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D21" s="4" t="str">
+        <f>'Raw Data'!C13</f>
         <v>Acme Rockets</v>
       </c>
-      <c r="E13" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E21" s="4" t="str">
+        <f>'Raw Data'!$BS$13</f>
         <v>500ml Red Wine</v>
       </c>
-      <c r="F13" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F21" s="4" t="str">
+        <f>'Raw Data'!$BT$13</f>
         <v>500ml Red Wine Van der Berg</v>
       </c>
-      <c r="G13" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I13" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+      <c r="G21" s="4" t="str">
+        <f>'Raw Data'!$CX$13</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H21" s="4" t="str">
+        <f>'Raw Data'!$BQ$13</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I21" s="5">
+        <f>'Raw Data'!$CC$13</f>
         <v>1</v>
       </c>
-      <c r="J13" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>16</v>
-      </c>
-      <c r="K13" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="J21" s="4" t="str">
+        <f>'Raw Data'!$AR$13</f>
         <v/>
       </c>
+      <c r="K21" s="4" t="str">
+        <f>'Raw Data'!$V$13</f>
+        <v/>
+      </c>
+      <c r="L21" s="4" t="str">
+        <f>'Raw Data'!$R$13</f>
+        <v>2021-01-13 00:00:00</v>
+      </c>
+      <c r="M21" s="4" t="str">
+        <f>'Raw Data'!$AQ$13</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="22" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="5">
+        <f>SUBTOTAL(9,I20:I21)</f>
+        <v>2</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="str">
+        <f>'Raw Data'!$G$14</f>
         <v>2020-10-07 00:00:00</v>
       </c>
-      <c r="B14" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>162</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B23" s="4">
+        <f>'Raw Data'!$BN$14</f>
+        <v>251</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f>'Raw Data'!$T$14</f>
         <v>2020-11-06 00:00:00</v>
       </c>
-      <c r="D14" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D23" s="4" t="str">
+        <f>'Raw Data'!C14</f>
         <v>Kidman</v>
       </c>
-      <c r="E14" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E23" s="4" t="str">
+        <f>'Raw Data'!$BS$14</f>
         <v>Monitor 607</v>
       </c>
-      <c r="F14" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F23" s="4" t="str">
+        <f>'Raw Data'!$BT$14</f>
         <v>Asus Monitor 607</v>
       </c>
-      <c r="G14" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I14" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>99</v>
-      </c>
-      <c r="K14" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G23" s="4" t="str">
+        <f>'Raw Data'!$CX$14</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H23" s="4" t="str">
+        <f>'Raw Data'!$BQ$14</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I23" s="5">
+        <f>'Raw Data'!$CC$14</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="str">
+        <f>'Raw Data'!$AR$14</f>
         <v>Approved for Invoicing</v>
       </c>
+      <c r="K23" s="4" t="str">
+        <f>'Raw Data'!$V$14</f>
+        <v>Back Order</v>
+      </c>
+      <c r="L23" s="4" t="str">
+        <f>'Raw Data'!$R$14</f>
+        <v>2020-10-07 00:00:00</v>
+      </c>
+      <c r="M23" s="4" t="str">
+        <f>'Raw Data'!$AQ$14</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="24" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="str">
+        <f>'Raw Data'!$G$15</f>
         <v>2020-10-07 00:00:00</v>
       </c>
-      <c r="B15" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>162</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B24" s="4">
+        <f>'Raw Data'!$BN$15</f>
+        <v>252</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <f>'Raw Data'!$T$15</f>
         <v>2020-11-06 00:00:00</v>
       </c>
-      <c r="D15" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D24" s="4" t="str">
+        <f>'Raw Data'!C15</f>
         <v>Kidman</v>
       </c>
-      <c r="E15" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E24" s="4" t="str">
+        <f>'Raw Data'!$BS$15</f>
         <v>PC Mouse</v>
       </c>
-      <c r="F15" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F24" s="4" t="str">
+        <f>'Raw Data'!$BT$15</f>
         <v>PC Mouse Black</v>
       </c>
-      <c r="G15" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I15" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>20</v>
-      </c>
-      <c r="K15" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G24" s="4" t="str">
+        <f>'Raw Data'!$CX$15</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f>'Raw Data'!$BQ$15</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I24" s="5">
+        <f>'Raw Data'!$CC$15</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="4" t="str">
+        <f>'Raw Data'!$AR$15</f>
         <v>Approved for Invoicing</v>
       </c>
+      <c r="K24" s="4" t="str">
+        <f>'Raw Data'!$V$15</f>
+        <v>Back Order</v>
+      </c>
+      <c r="L24" s="4" t="str">
+        <f>'Raw Data'!$R$15</f>
+        <v>2020-10-07 00:00:00</v>
+      </c>
+      <c r="M24" s="4" t="str">
+        <f>'Raw Data'!$AQ$15</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="25" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="str">
+        <f>'Raw Data'!$G$16</f>
         <v>2020-10-07 00:00:00</v>
       </c>
-      <c r="B16" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>162</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B25" s="4">
+        <f>'Raw Data'!$BN$16</f>
+        <v>253</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f>'Raw Data'!$T$16</f>
         <v>2020-11-06 00:00:00</v>
       </c>
-      <c r="D16" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D25" s="4" t="str">
+        <f>'Raw Data'!C16</f>
         <v>Kidman</v>
       </c>
-      <c r="E16" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E25" s="4" t="str">
+        <f>'Raw Data'!$BS$16</f>
         <v>Keyboard</v>
       </c>
-      <c r="F16" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F25" s="4" t="str">
+        <f>'Raw Data'!$BT$16</f>
         <v>Keyboard Black</v>
       </c>
-      <c r="G16" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I16" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>10</v>
-      </c>
-      <c r="K16" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G25" s="4" t="str">
+        <f>'Raw Data'!$CX$16</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H25" s="4" t="str">
+        <f>'Raw Data'!$BQ$16</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I25" s="5">
+        <f>'Raw Data'!$CC$16</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4" t="str">
+        <f>'Raw Data'!$AR$16</f>
         <v>Approved for Invoicing</v>
       </c>
+      <c r="K25" s="4" t="str">
+        <f>'Raw Data'!$V$16</f>
+        <v>Back Order</v>
+      </c>
+      <c r="L25" s="4" t="str">
+        <f>'Raw Data'!$R$16</f>
+        <v>2020-10-07 00:00:00</v>
+      </c>
+      <c r="M25" s="4" t="str">
+        <f>'Raw Data'!$AQ$16</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="26" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="str">
+        <f>'Raw Data'!$G$17</f>
         <v>2020-10-07 00:00:00</v>
       </c>
-      <c r="B17" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>162</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B26" s="4">
+        <f>'Raw Data'!$BN$17</f>
+        <v>254</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f>'Raw Data'!$T$17</f>
         <v>2020-11-06 00:00:00</v>
       </c>
-      <c r="D17" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D26" s="4" t="str">
+        <f>'Raw Data'!C17</f>
         <v>Kidman</v>
       </c>
-      <c r="E17" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E26" s="4" t="str">
+        <f>'Raw Data'!$BS$17</f>
         <v>Mouse Pad</v>
       </c>
-      <c r="F17" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F26" s="4" t="str">
+        <f>'Raw Data'!$BT$17</f>
         <v>Garfield Mouse Pad</v>
       </c>
-      <c r="G17" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I17" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>20</v>
-      </c>
-      <c r="K17" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G26" s="4" t="str">
+        <f>'Raw Data'!$CX$17</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H26" s="4" t="str">
+        <f>'Raw Data'!$BQ$17</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I26" s="5">
+        <f>'Raw Data'!$CC$17</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="4" t="str">
+        <f>'Raw Data'!$AR$17</f>
         <v>Approved for Invoicing</v>
       </c>
+      <c r="K26" s="4" t="str">
+        <f>'Raw Data'!$V$17</f>
+        <v>Back Order</v>
+      </c>
+      <c r="L26" s="4" t="str">
+        <f>'Raw Data'!$R$17</f>
+        <v>2020-10-07 00:00:00</v>
+      </c>
+      <c r="M26" s="4" t="str">
+        <f>'Raw Data'!$AQ$17</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="27" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="5">
+        <f>SUBTOTAL(9,I23:I26)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="str">
+        <f>'Raw Data'!$G$18</f>
         <v>2020-09-30 00:00:00</v>
       </c>
-      <c r="B18" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>38</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
+      <c r="B28" s="4">
+        <f>'Raw Data'!$BN$18</f>
+        <v>82</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <f>'Raw Data'!$T$18</f>
         <v>2020-09-17 00:00:00</v>
       </c>
-      <c r="D18" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
+      <c r="D28" s="4" t="str">
+        <f>'Raw Data'!C18</f>
         <v>Telco 3</v>
       </c>
-      <c r="E18" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
+      <c r="E28" s="4" t="str">
+        <f>'Raw Data'!$BS$18</f>
         <v>Office Chair</v>
       </c>
-      <c r="F18" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
+      <c r="F28" s="4" t="str">
+        <f>'Raw Data'!$BT$18</f>
         <v>Leather Office Chair</v>
       </c>
-      <c r="G18" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I18" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>12</v>
-      </c>
-      <c r="K18" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="G28" s="4" t="str">
+        <f>'Raw Data'!$CX$18</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H28" s="4" t="str">
+        <f>'Raw Data'!$BQ$18</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I28" s="5">
+        <f>'Raw Data'!$CC$18</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="4" t="str">
+        <f>'Raw Data'!$AR$18</f>
         <v>Prepared</v>
       </c>
+      <c r="K28" s="4" t="str">
+        <f>'Raw Data'!$V$18</f>
+        <v>Prepared</v>
+      </c>
+      <c r="L28" s="4" t="str">
+        <f>'Raw Data'!$R$18</f>
+        <v>2020-09-03 00:00:00</v>
+      </c>
+      <c r="M28" s="4" t="str">
+        <f>'Raw Data'!$AQ$18</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
+    <row r="29" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="5">
+        <f>SUBTOTAL(9,I28:I28)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="str">
+        <f>'Raw Data'!$G$19</f>
         <v>2020-08-05 00:00:00</v>
       </c>
-      <c r="B19" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
+      <c r="B30" s="4">
+        <f>'Raw Data'!$BN$19</f>
+        <v>80</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <f>'Raw Data'!$T$19</f>
+        <v>2020-08-12 00:00:00</v>
+      </c>
+      <c r="D30" s="4" t="str">
+        <f>'Raw Data'!C19</f>
+        <v>Jones</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <f>'Raw Data'!$BS$19</f>
+        <v>PC Mouse</v>
+      </c>
+      <c r="F30" s="4" t="str">
+        <f>'Raw Data'!$BT$19</f>
+        <v>PC Mouse Black</v>
+      </c>
+      <c r="G30" s="4" t="str">
+        <f>'Raw Data'!$CX$19</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H30" s="4" t="str">
+        <f>'Raw Data'!$BQ$19</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I30" s="5">
+        <f>'Raw Data'!$CC$19</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="4" t="str">
+        <f>'Raw Data'!$AR$19</f>
+        <v>Approved</v>
+      </c>
+      <c r="K30" s="4" t="str">
+        <f>'Raw Data'!$V$19</f>
+        <v>Awaiting</v>
+      </c>
+      <c r="L30" s="4" t="str">
+        <f>'Raw Data'!$R$19</f>
+        <v>2020-08-05 00:00:00</v>
+      </c>
+      <c r="M30" s="4" t="str">
+        <f>'Raw Data'!$AQ$19</f>
+        <v>Sample Company</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="5">
+        <f>SUBTOTAL(9,I30:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="str">
+        <f>'Raw Data'!$G$20</f>
+        <v>2020-09-03 00:00:00</v>
+      </c>
+      <c r="B32" s="4">
+        <f>'Raw Data'!$BN$20</f>
         <v>37</v>
       </c>
-      <c r="C19" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
-        <v>2020-08-12 00:00:00</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
-        <v>Jones</v>
-      </c>
-      <c r="E19" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
-        <v>PC Mouse</v>
-      </c>
-      <c r="F19" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
-        <v>PC Mouse Black</v>
-      </c>
-      <c r="G19" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I19" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>20</v>
-      </c>
-      <c r="K19" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
+      <c r="C32" s="4" t="str">
+        <f>'Raw Data'!$T$20</f>
+        <v>2020-09-17 00:00:00</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <f>'Raw Data'!C20</f>
+        <v>Voss</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <f>'Raw Data'!$BS$20</f>
+        <v>500ml Red Wine</v>
+      </c>
+      <c r="F32" s="4" t="str">
+        <f>'Raw Data'!$BT$20</f>
+        <v>500ml Red Wine Van der Berg</v>
+      </c>
+      <c r="G32" s="4" t="str">
+        <f>'Raw Data'!$CX$20</f>
+        <v>1899-12-30 00:00:00</v>
+      </c>
+      <c r="H32" s="4" t="str">
+        <f>'Raw Data'!$BQ$20</f>
+        <v>Inventory Asset</v>
+      </c>
+      <c r="I32" s="5">
+        <f>'Raw Data'!$CC$20</f>
+        <v>5</v>
+      </c>
+      <c r="J32" s="4" t="str">
+        <f>'Raw Data'!$AR$20</f>
+        <v>Approved for Invoicing</v>
+      </c>
+      <c r="K32" s="4" t="str">
+        <f>'Raw Data'!$V$20</f>
         <v>Approved</v>
       </c>
+      <c r="L32" s="4" t="str">
+        <f>'Raw Data'!$R$20</f>
+        <v>2020-09-03 00:00:00</v>
+      </c>
+      <c r="M32" s="4" t="str">
+        <f>'Raw Data'!$AQ$20</f>
+        <v>Sample Company</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.SaleDate]]</f>
-        <v>2020-09-03 00:00:00</v>
-      </c>
-      <c r="B20" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.InvoiceDocNumber]]</f>
-        <v>17</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.DueDate]]</f>
-        <v>2020-09-17 00:00:00</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.CustomerName]]</f>
-        <v>Voss</v>
-      </c>
-      <c r="E20" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.ProductName]]</f>
-        <v>500ml Red Wine</v>
-      </c>
-      <c r="F20" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.Product_Description]]</f>
-        <v>500ml Red Wine Van der Berg</v>
-      </c>
-      <c r="G20" s="3">
-        <v>44928</v>
-      </c>
-      <c r="I20" s="2">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QtySold]]</f>
+    <row r="33" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="5">
+        <f>SUBTOTAL(9,I32:I32)</f>
         <v>5</v>
       </c>
-      <c r="J20" s="4">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.LineCost]]</f>
-        <v>16</v>
-      </c>
-      <c r="K20" s="2" t="str">
-        <f>TInvoiceList_IgnoreDates_true_Search_Deleted_20__3D_20true_OrderBy_SaleID_20desc[[#This Row],[T.QuoteStatus]]</f>
-        <v>Approved for Invoicing</v>
-      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="5">
+        <f>SUBTOTAL(9,I2:I32)</f>
+        <v>53</v>
+      </c>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A51A1F9-6E19-44F0-909E-980309D07BD6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ20"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>

</xml_diff>